<commit_message>
Art station upload and fixed asset list
</commit_message>
<xml_diff>
--- a/Asset List:Schedule.xlsx
+++ b/Asset List:Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbinwalker/Documents/Digital Media/DGM-3650/Asset List:"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360C219A-32D6-A243-8567-62FC92FD3450}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51EAECA-F878-6D4D-9377-BEB4FC3DB06D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="460" windowWidth="27820" windowHeight="17040" activeTab="1" xr2:uid="{8439A946-5B6C-3D45-A729-A84689364E52}"/>
   </bookViews>
@@ -254,9 +254,6 @@
     <t>December</t>
   </si>
   <si>
-    <t>End of th semester</t>
-  </si>
-  <si>
     <t>Dec 04, 2018</t>
   </si>
   <si>
@@ -294,6 +291,9 @@
   </si>
   <si>
     <t>and back completed</t>
+  </si>
+  <si>
+    <t>End of the semester</t>
   </si>
 </sst>
 </file>
@@ -3729,7 +3729,7 @@
       <c r="P4" s="6"/>
       <c r="R4" s="6"/>
       <c r="T4" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
@@ -3754,7 +3754,7 @@
       <c r="P5" s="6"/>
       <c r="R5" s="6"/>
       <c r="T5" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
@@ -3779,7 +3779,7 @@
       <c r="P6" s="6"/>
       <c r="R6" s="6"/>
       <c r="T6" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
@@ -3829,7 +3829,7 @@
       <c r="P8" s="6"/>
       <c r="R8" s="6"/>
       <c r="T8" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
@@ -3854,7 +3854,7 @@
       <c r="P9" s="6"/>
       <c r="R9" s="6"/>
       <c r="T9" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
@@ -3913,7 +3913,7 @@
       <c r="P11" s="6"/>
       <c r="R11" s="6"/>
       <c r="T11" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
@@ -3938,7 +3938,7 @@
       <c r="P12" s="6"/>
       <c r="R12" s="6"/>
       <c r="T12" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="V12" s="6"/>
       <c r="W12" s="6"/>
@@ -3963,7 +3963,7 @@
       <c r="P13" s="6"/>
       <c r="R13" s="6"/>
       <c r="T13" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
@@ -3988,7 +3988,7 @@
       <c r="P14" s="6"/>
       <c r="R14" s="6"/>
       <c r="T14" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
@@ -4013,7 +4013,7 @@
       <c r="P15" s="6"/>
       <c r="R15" s="6"/>
       <c r="T15" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V15" s="6"/>
       <c r="W15" s="6"/>
@@ -4624,7 +4624,7 @@
       <c r="P38" s="6"/>
       <c r="R38" s="6"/>
       <c r="T38" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V38" s="6"/>
       <c r="W38" s="6"/>
@@ -4649,7 +4649,7 @@
       <c r="P39" s="6"/>
       <c r="R39" s="6"/>
       <c r="T39" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V39" s="6"/>
       <c r="W39" s="6"/>
@@ -4674,7 +4674,7 @@
       <c r="P40" s="6"/>
       <c r="R40" s="6"/>
       <c r="T40" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V40" s="6"/>
       <c r="W40" s="6"/>
@@ -4699,7 +4699,7 @@
       <c r="P41" s="6"/>
       <c r="R41" s="6"/>
       <c r="T41" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V41" s="6"/>
       <c r="W41" s="6"/>
@@ -4724,7 +4724,7 @@
       <c r="P42" s="6"/>
       <c r="R42" s="6"/>
       <c r="T42" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V42" s="6"/>
       <c r="W42" s="6"/>
@@ -4738,7 +4738,7 @@
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -4783,7 +4783,7 @@
       <c r="P44" s="6"/>
       <c r="R44" s="6"/>
       <c r="T44" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V44" s="6"/>
       <c r="W44" s="6"/>
@@ -4808,7 +4808,7 @@
       <c r="P45" s="6"/>
       <c r="R45" s="6"/>
       <c r="T45" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V45" s="6"/>
       <c r="W45" s="6"/>
@@ -4833,7 +4833,7 @@
       <c r="P46" s="6"/>
       <c r="R46" s="6"/>
       <c r="T46" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V46" s="6"/>
       <c r="W46" s="6"/>
@@ -4858,7 +4858,7 @@
       <c r="P47" s="6"/>
       <c r="R47" s="6"/>
       <c r="T47" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V47" s="6"/>
       <c r="W47" s="6"/>
@@ -5746,7 +5746,7 @@
   <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6391,7 +6391,7 @@
       <c r="F37" s="20"/>
       <c r="G37" s="20"/>
       <c r="H37" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I37" s="21"/>
       <c r="J37" s="20"/>
@@ -6521,7 +6521,7 @@
       <c r="F43" s="20"/>
       <c r="G43" s="20"/>
       <c r="H43" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I43" s="21"/>
       <c r="J43" s="20"/>
@@ -6539,7 +6539,7 @@
       <c r="F44" s="20"/>
       <c r="G44" s="20"/>
       <c r="H44" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I44" s="21"/>
       <c r="J44" s="20"/>
@@ -6587,7 +6587,7 @@
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
       <c r="H46" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I46" s="20"/>
       <c r="J46" s="21"/>
@@ -6605,7 +6605,7 @@
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
       <c r="H47" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I47" s="20"/>
       <c r="J47" s="21"/>
@@ -6680,7 +6680,7 @@
       <c r="F54" s="23"/>
       <c r="G54" s="23"/>
       <c r="H54" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I54" s="24"/>
       <c r="J54" s="23"/>
@@ -6726,7 +6726,7 @@
       <c r="D57" s="23"/>
       <c r="E57" s="23"/>
       <c r="F57" s="25" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="G57" s="24"/>
     </row>

</xml_diff>

<commit_message>
Both modern and Og Parthenon Vr models made and imported
</commit_message>
<xml_diff>
--- a/Asset List:Schedule.xlsx
+++ b/Asset List:Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbinwalker/Documents/Digital Media/DGM-3650/Asset List:"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51EAECA-F878-6D4D-9377-BEB4FC3DB06D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9409F4FF-BDF0-0347-B832-F5F74736DE44}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="460" windowWidth="27820" windowHeight="17040" activeTab="1" xr2:uid="{8439A946-5B6C-3D45-A729-A84689364E52}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="93">
   <si>
     <t>Asset List</t>
   </si>
@@ -230,9 +230,6 @@
     <t>October</t>
   </si>
   <si>
-    <t>Scripting/UI Completed</t>
-  </si>
-  <si>
     <t>Begin Modeling/</t>
   </si>
   <si>
@@ -245,9 +242,6 @@
     <t>Oct 11,2018</t>
   </si>
   <si>
-    <t>Sound Completed</t>
-  </si>
-  <si>
     <t>November</t>
   </si>
   <si>
@@ -260,9 +254,6 @@
     <t>Oct 25, 2018</t>
   </si>
   <si>
-    <t>Parthenon modern</t>
-  </si>
-  <si>
     <t>Nov 04, 2018</t>
   </si>
   <si>
@@ -294,6 +285,27 @@
   </si>
   <si>
     <t>End of the semester</t>
+  </si>
+  <si>
+    <t>Ancient Parthenon WB</t>
+  </si>
+  <si>
+    <t>Modern Parhtenon WB</t>
+  </si>
+  <si>
+    <t>Statue of Athena WB</t>
+  </si>
+  <si>
+    <t>put into VR and Also</t>
+  </si>
+  <si>
+    <t>scaled in Vr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simple Ui created for </t>
+  </si>
+  <si>
+    <t>Play testing</t>
   </si>
 </sst>
 </file>
@@ -486,7 +498,7 @@
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="5"/>
@@ -515,6 +527,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="12" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="15" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="16" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="7" applyFont="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -3622,7 +3635,7 @@
   <dimension ref="A1:AD47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T38" sqref="T38:T42"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3729,7 +3742,7 @@
       <c r="P4" s="6"/>
       <c r="R4" s="6"/>
       <c r="T4" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
@@ -3754,7 +3767,7 @@
       <c r="P5" s="6"/>
       <c r="R5" s="6"/>
       <c r="T5" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
@@ -3779,7 +3792,7 @@
       <c r="P6" s="6"/>
       <c r="R6" s="6"/>
       <c r="T6" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
@@ -3829,7 +3842,7 @@
       <c r="P8" s="6"/>
       <c r="R8" s="6"/>
       <c r="T8" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
@@ -3854,7 +3867,7 @@
       <c r="P9" s="6"/>
       <c r="R9" s="6"/>
       <c r="T9" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
@@ -3913,7 +3926,7 @@
       <c r="P11" s="6"/>
       <c r="R11" s="6"/>
       <c r="T11" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
@@ -3938,7 +3951,7 @@
       <c r="P12" s="6"/>
       <c r="R12" s="6"/>
       <c r="T12" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="V12" s="6"/>
       <c r="W12" s="6"/>
@@ -3963,7 +3976,7 @@
       <c r="P13" s="6"/>
       <c r="R13" s="6"/>
       <c r="T13" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
@@ -3988,7 +4001,7 @@
       <c r="P14" s="6"/>
       <c r="R14" s="6"/>
       <c r="T14" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
@@ -4013,7 +4026,7 @@
       <c r="P15" s="6"/>
       <c r="R15" s="6"/>
       <c r="T15" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="V15" s="6"/>
       <c r="W15" s="6"/>
@@ -4072,7 +4085,7 @@
       <c r="P17" s="6"/>
       <c r="R17" s="6"/>
       <c r="T17" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
@@ -4097,7 +4110,7 @@
       <c r="P18" s="6"/>
       <c r="R18" s="6"/>
       <c r="T18" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
@@ -4122,7 +4135,7 @@
       <c r="P19" s="6"/>
       <c r="R19" s="6"/>
       <c r="T19" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
@@ -4147,7 +4160,7 @@
       <c r="P20" s="6"/>
       <c r="R20" s="6"/>
       <c r="T20" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V20" s="6"/>
       <c r="W20" s="6"/>
@@ -4172,7 +4185,7 @@
       <c r="P21" s="6"/>
       <c r="R21" s="6"/>
       <c r="T21" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
@@ -4231,7 +4244,7 @@
       <c r="P23" s="6"/>
       <c r="R23" s="6"/>
       <c r="T23" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
@@ -4256,7 +4269,7 @@
       <c r="P24" s="6"/>
       <c r="R24" s="6"/>
       <c r="T24" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
@@ -4281,7 +4294,7 @@
       <c r="P25" s="6"/>
       <c r="R25" s="6"/>
       <c r="T25" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
@@ -4306,7 +4319,7 @@
       <c r="P26" s="6"/>
       <c r="R26" s="6"/>
       <c r="T26" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
@@ -4331,7 +4344,7 @@
       <c r="P27" s="6"/>
       <c r="R27" s="6"/>
       <c r="T27" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V27" s="6"/>
       <c r="W27" s="6"/>
@@ -4356,7 +4369,7 @@
       <c r="P28" s="6"/>
       <c r="R28" s="6"/>
       <c r="T28" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V28" s="6"/>
       <c r="W28" s="6"/>
@@ -4381,7 +4394,7 @@
       <c r="P29" s="6"/>
       <c r="R29" s="6"/>
       <c r="T29" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V29" s="6"/>
       <c r="W29" s="6"/>
@@ -4406,7 +4419,7 @@
       <c r="P30" s="6"/>
       <c r="R30" s="6"/>
       <c r="T30" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V30" s="6"/>
       <c r="W30" s="6"/>
@@ -4624,7 +4637,7 @@
       <c r="P38" s="6"/>
       <c r="R38" s="6"/>
       <c r="T38" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="V38" s="6"/>
       <c r="W38" s="6"/>
@@ -4649,7 +4662,7 @@
       <c r="P39" s="6"/>
       <c r="R39" s="6"/>
       <c r="T39" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="V39" s="6"/>
       <c r="W39" s="6"/>
@@ -4674,7 +4687,7 @@
       <c r="P40" s="6"/>
       <c r="R40" s="6"/>
       <c r="T40" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="V40" s="6"/>
       <c r="W40" s="6"/>
@@ -4699,7 +4712,7 @@
       <c r="P41" s="6"/>
       <c r="R41" s="6"/>
       <c r="T41" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="V41" s="6"/>
       <c r="W41" s="6"/>
@@ -4724,7 +4737,7 @@
       <c r="P42" s="6"/>
       <c r="R42" s="6"/>
       <c r="T42" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="V42" s="6"/>
       <c r="W42" s="6"/>
@@ -4738,7 +4751,7 @@
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -4783,7 +4796,7 @@
       <c r="P44" s="6"/>
       <c r="R44" s="6"/>
       <c r="T44" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="V44" s="6"/>
       <c r="W44" s="6"/>
@@ -4808,7 +4821,7 @@
       <c r="P45" s="6"/>
       <c r="R45" s="6"/>
       <c r="T45" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="V45" s="6"/>
       <c r="W45" s="6"/>
@@ -4833,7 +4846,7 @@
       <c r="P46" s="6"/>
       <c r="R46" s="6"/>
       <c r="T46" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="V46" s="6"/>
       <c r="W46" s="6"/>
@@ -4858,7 +4871,7 @@
       <c r="P47" s="6"/>
       <c r="R47" s="6"/>
       <c r="T47" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="V47" s="6"/>
       <c r="W47" s="6"/>
@@ -5745,8 +5758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F8186B-541E-CB41-B7D3-31AE7BE22136}">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5841,7 +5854,7 @@
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K6" s="10"/>
       <c r="L6" s="11"/>
@@ -5859,7 +5872,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="11"/>
@@ -6162,7 +6175,7 @@
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
       <c r="H23" s="17" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="I23" s="15"/>
       <c r="J23" s="16"/>
@@ -6179,7 +6192,9 @@
       <c r="E24" s="15"/>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="17" t="s">
+        <v>52</v>
+      </c>
       <c r="I24" s="15"/>
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
@@ -6225,8 +6240,8 @@
       <c r="E26" s="16"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
-      <c r="H26" s="16" t="s">
-        <v>67</v>
+      <c r="H26" s="28" t="s">
+        <v>87</v>
       </c>
       <c r="I26" s="16"/>
       <c r="J26" s="15"/>
@@ -6243,7 +6258,9 @@
       <c r="E27" s="16"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
-      <c r="H27" s="16"/>
+      <c r="H27" s="28" t="s">
+        <v>52</v>
+      </c>
       <c r="I27" s="16"/>
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
@@ -6290,7 +6307,7 @@
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="17" t="s">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="I29" s="15"/>
       <c r="J29" s="16"/>
@@ -6350,7 +6367,7 @@
     </row>
     <row r="35" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="2:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -6391,7 +6408,7 @@
       <c r="F37" s="20"/>
       <c r="G37" s="20"/>
       <c r="H37" s="26" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="I37" s="21"/>
       <c r="J37" s="20"/>
@@ -6409,7 +6426,7 @@
       <c r="F38" s="20"/>
       <c r="G38" s="20"/>
       <c r="H38" s="26" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="I38" s="21"/>
       <c r="J38" s="20"/>
@@ -6457,7 +6474,7 @@
       <c r="F40" s="21"/>
       <c r="G40" s="21"/>
       <c r="H40" s="27" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="I40" s="20"/>
       <c r="J40" s="21"/>
@@ -6474,7 +6491,9 @@
       <c r="E41" s="20"/>
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
-      <c r="H41" s="20"/>
+      <c r="H41" s="27" t="s">
+        <v>92</v>
+      </c>
       <c r="I41" s="20"/>
       <c r="J41" s="21"/>
       <c r="K41" s="21"/>
@@ -6521,7 +6540,7 @@
       <c r="F43" s="20"/>
       <c r="G43" s="20"/>
       <c r="H43" s="26" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I43" s="21"/>
       <c r="J43" s="20"/>
@@ -6539,7 +6558,7 @@
       <c r="F44" s="20"/>
       <c r="G44" s="20"/>
       <c r="H44" s="26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I44" s="21"/>
       <c r="J44" s="20"/>
@@ -6587,7 +6606,7 @@
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
       <c r="H46" s="27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I46" s="20"/>
       <c r="J46" s="21"/>
@@ -6605,7 +6624,7 @@
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
       <c r="H47" s="27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I47" s="20"/>
       <c r="J47" s="21"/>
@@ -6639,7 +6658,7 @@
     </row>
     <row r="52" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="2:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -6680,7 +6699,7 @@
       <c r="F54" s="23"/>
       <c r="G54" s="23"/>
       <c r="H54" s="25" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I54" s="24"/>
       <c r="J54" s="23"/>
@@ -6726,7 +6745,7 @@
       <c r="D57" s="23"/>
       <c r="E57" s="23"/>
       <c r="F57" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G57" s="24"/>
     </row>

</xml_diff>